<commit_message>
Updated OC RR and fixed xlrd error
</commit_message>
<xml_diff>
--- a/data/model_inputs.xlsx
+++ b/data/model_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisabethsilver/Documents/project_lynch_syndrome_gyn/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4579FB0-3B46-F644-AE7B-ECFDF4A19FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49ECE99-9833-5344-BE02-5E3D0E8AE3E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16260" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16260" firstSheet="6" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="performance_chars" sheetId="1" r:id="rId1"/>
@@ -4294,8 +4294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4356,17 +4356,17 @@
         <v>82</v>
       </c>
       <c r="B3">
-        <v>0.66</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0.51</v>
+        <v>0.85</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
         <f>0.2*B3</f>
-        <v>0.13200000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F3" t="s">
         <v>125</v>
@@ -9142,7 +9142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>

</xml_diff>